<commit_message>
Reverted to commit 4590c3118d16b4edc5b2199cf6c03cd35dbce3c3
</commit_message>
<xml_diff>
--- a/Análisis_del_archivo_BASE_DE_DADOS_CSV-Genspark_AI_Sheets-20260130_2001.xlsx
+++ b/Análisis_del_archivo_BASE_DE_DADOS_CSV-Genspark_AI_Sheets-20260130_2001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c501bd79870a90b3/Área de Trabalho/GRUPO DOCTOR/doctorautoprime/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{4AD85B73-9105-4D3F-B7F2-FCF628D4DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C638813-63FD-4DB6-92EA-3B11E0F2989F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4AD85B73-9105-4D3F-B7F2-FCF628D4DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00_EMPRESAS" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="16_PECAS_SERVICOS_NAO_EXECUTADO" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -642,7 +643,7 @@
     <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="169" formatCode="[$R$-416]\ #,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,13 +671,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -794,15 +788,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -922,10 +913,8 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -939,6 +928,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1232,7 +1225,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17659,7 +17652,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17669,7 +17662,7 @@
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="21.44140625" customWidth="1"/>
@@ -28954,7 +28947,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -29055,9 +29048,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF583338-8DE8-8BBD-51E8-A2DF490D40E5}">
   <dimension ref="A1:AM100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -29125,7 +29118,7 @@
       <c r="D2" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="17" t="s">
         <v>87</v>
       </c>
       <c r="F2" s="18" t="s">
@@ -30548,9 +30541,6 @@
       <c r="L100" s="20"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{517E2F97-C80B-4206-81A4-574EF0497624}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -30564,7 +30554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D91A176-6F8E-E3D8-88AE-8CD15FD9BB3E}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>